<commit_message>
working on manuscript for New Phytologist
</commit_message>
<xml_diff>
--- a/data/PlantingData.xlsx
+++ b/data/PlantingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED84E61-FE8B-4CE1-843D-F5EB0C469D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAAC23F-FC16-490C-874F-611CC08384C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FFAFF3EB-B419-47E1-98F1-7FCFAB378E2D}"/>
+    <workbookView xWindow="3132" yWindow="1872" windowWidth="17280" windowHeight="8964" xr2:uid="{FFAFF3EB-B419-47E1-98F1-7FCFAB378E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sporophytic" sheetId="1" r:id="rId1"/>
@@ -618,9 +618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C2BDB9-DDA1-4456-B96B-B7C6BC14A59C}">
   <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4465,7 +4465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E5F978-1CB9-4F8E-A0CD-EE0A5A02EA8E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>